<commit_message>
removed threading and added new
</commit_message>
<xml_diff>
--- a/swap_request_log.xlsx
+++ b/swap_request_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="36">
   <si>
     <t>Requester_ID</t>
   </si>
@@ -98,6 +98,30 @@
   </si>
   <si>
     <t>2024-05-21 10:24:17</t>
+  </si>
+  <si>
+    <t>2024-05-21 16:02:47</t>
+  </si>
+  <si>
+    <t>2024-05-21 18:23:41</t>
+  </si>
+  <si>
+    <t>2024-05-22 17:21:01</t>
+  </si>
+  <si>
+    <t>2024-05-22 17:25:05</t>
+  </si>
+  <si>
+    <t>2024-05-22 17:29:04</t>
+  </si>
+  <si>
+    <t>2024-05-22 18:23:08</t>
+  </si>
+  <si>
+    <t>2024-05-22 22:08:40</t>
+  </si>
+  <si>
+    <t>2024-05-22 22:27:07</t>
   </si>
 </sst>
 </file>
@@ -455,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -808,6 +832,238 @@
         <v>27</v>
       </c>
     </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>